<commit_message>
Updates to reflect multi-copy gene placement
Removed three genes from KMA due to NNN stretches in FASTA file. KMA analysis will be rerun to reflec this.
</commit_message>
<xml_diff>
--- a/Figure3 and Supplement3/cpk/Cen.PK_RNA_DE_OrthologyMatching.xlsx
+++ b/Figure3 and Supplement3/cpk/Cen.PK_RNA_DE_OrthologyMatching.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doughty/Documents/GitHub/CHASSY_multiOmics_Analysis/Figure3 and Supplement3/cpk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F43F22-015E-4C4C-8027-BC1E1F9736A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE242030-A650-DB4A-A4F6-AE5D97950217}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36900" yWindow="2400" windowWidth="30980" windowHeight="18400" xr2:uid="{96708D6E-F787-8A40-A70C-D04BD086EDC7}"/>
+    <workbookView xWindow="-34400" yWindow="3120" windowWidth="30980" windowHeight="18400" activeTab="2" xr2:uid="{96708D6E-F787-8A40-A70C-D04BD086EDC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cen.PK_HiT_Significant" sheetId="1" r:id="rId1"/>
     <sheet name="Cen.PK_LpH_Significant" sheetId="2" r:id="rId2"/>
     <sheet name="Cen.PK_Osm_Significant" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="580">
   <si>
     <t>genes</t>
   </si>
@@ -1767,12 +1767,6 @@
   </si>
   <si>
     <t>CPK Low PH DE RNA Analysis</t>
-  </si>
-  <si>
-    <t>DE mRNAs</t>
-  </si>
-  <si>
-    <t>Total mRNAs</t>
   </si>
 </sst>
 </file>
@@ -2125,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D4289B-7807-0047-82A7-AF7BADD90F28}">
-  <dimension ref="A1:N149"/>
+  <dimension ref="A1:M149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="F14:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2138,7 +2132,7 @@
     <col min="8" max="8" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2146,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2194,7 +2188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2208,7 +2202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2221,11 +2215,8 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2238,23 +2229,8 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
-        <v>572</v>
-      </c>
-      <c r="I7" t="s">
-        <v>573</v>
-      </c>
-      <c r="J7" t="s">
-        <v>574</v>
-      </c>
-      <c r="K7" t="s">
-        <v>575</v>
-      </c>
-      <c r="L7" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2267,26 +2243,8 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2299,29 +2257,8 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" t="s">
-        <v>578</v>
-      </c>
-      <c r="H9">
-        <v>59</v>
-      </c>
-      <c r="I9">
-        <v>37</v>
-      </c>
-      <c r="J9">
-        <v>19</v>
-      </c>
-      <c r="K9">
-        <v>16</v>
-      </c>
-      <c r="L9">
-        <v>17</v>
-      </c>
-      <c r="N9">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2334,29 +2271,8 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10">
-        <v>2580</v>
-      </c>
-      <c r="I10">
-        <v>1571</v>
-      </c>
-      <c r="J10">
-        <v>844</v>
-      </c>
-      <c r="K10">
-        <v>290</v>
-      </c>
-      <c r="L10">
-        <v>166</v>
-      </c>
-      <c r="N10">
-        <v>5451</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2369,29 +2285,8 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
-        <v>577</v>
-      </c>
-      <c r="H11">
-        <v>2.2868217054263567</v>
-      </c>
-      <c r="I11">
-        <v>2.3551877784850412</v>
-      </c>
-      <c r="J11">
-        <v>2.2511848341232228</v>
-      </c>
-      <c r="K11">
-        <v>5.5172413793103452</v>
-      </c>
-      <c r="L11">
-        <v>10.240963855421686</v>
-      </c>
-      <c r="N11">
-        <v>2.715098147128967</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2404,29 +2299,8 @@
       <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H12">
-        <v>0.84226115650534261</v>
-      </c>
-      <c r="I12">
-        <v>0.86744112030553788</v>
-      </c>
-      <c r="J12">
-        <v>0.82913571154092491</v>
-      </c>
-      <c r="K12">
-        <v>2.0320596458527493</v>
-      </c>
-      <c r="L12">
-        <v>3.7718577010745684</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2453,8 +2327,11 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2467,8 +2344,23 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>572</v>
+      </c>
+      <c r="H15" t="s">
+        <v>573</v>
+      </c>
+      <c r="I15" t="s">
+        <v>574</v>
+      </c>
+      <c r="J15" t="s">
+        <v>575</v>
+      </c>
+      <c r="K15" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2481,8 +2373,26 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2495,8 +2405,29 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>578</v>
+      </c>
+      <c r="G17">
+        <v>59</v>
+      </c>
+      <c r="H17">
+        <v>37</v>
+      </c>
+      <c r="I17">
+        <v>19</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>17</v>
+      </c>
+      <c r="M17">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2509,8 +2440,29 @@
       <c r="D18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18">
+        <v>2580</v>
+      </c>
+      <c r="H18">
+        <v>1635</v>
+      </c>
+      <c r="I18">
+        <v>780</v>
+      </c>
+      <c r="J18">
+        <v>290</v>
+      </c>
+      <c r="K18">
+        <v>166</v>
+      </c>
+      <c r="M18">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2523,8 +2475,29 @@
       <c r="D19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>577</v>
+      </c>
+      <c r="G19">
+        <v>2.2868217054263567</v>
+      </c>
+      <c r="H19">
+        <v>2.2629969418960245</v>
+      </c>
+      <c r="I19">
+        <v>2.4358974358974361</v>
+      </c>
+      <c r="J19">
+        <v>5.5172413793103452</v>
+      </c>
+      <c r="K19">
+        <v>10.240963855421686</v>
+      </c>
+      <c r="M19">
+        <v>2.715098147128967</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2537,8 +2510,29 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>328</v>
+      </c>
+      <c r="G20">
+        <v>0.84226115650534261</v>
+      </c>
+      <c r="H20">
+        <v>0.83348623853211012</v>
+      </c>
+      <c r="I20">
+        <v>0.89716735966735983</v>
+      </c>
+      <c r="J20">
+        <v>2.0320596458527493</v>
+      </c>
+      <c r="K20">
+        <v>3.7718577010745684</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2552,7 +2546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2566,7 +2560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2580,7 +2574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2594,7 +2588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2608,7 +2602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2622,7 +2616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2636,7 +2630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2650,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2664,7 +2658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2692,7 +2686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -4354,7 +4348,7 @@
   <dimension ref="A1:M219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="M23" sqref="F17:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4365,7 +4359,7 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4379,7 +4373,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -4393,7 +4387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -4407,7 +4401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -4421,7 +4415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -4435,7 +4429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -4449,7 +4443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -4463,7 +4457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -4476,11 +4470,8 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4493,23 +4484,8 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>572</v>
-      </c>
-      <c r="H9" t="s">
-        <v>573</v>
-      </c>
-      <c r="I9" t="s">
-        <v>574</v>
-      </c>
-      <c r="J9" t="s">
-        <v>575</v>
-      </c>
-      <c r="K9" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>166</v>
       </c>
@@ -4522,26 +4498,8 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>167</v>
       </c>
@@ -4554,29 +4512,8 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
-        <v>580</v>
-      </c>
-      <c r="G11">
-        <v>104</v>
-      </c>
-      <c r="H11">
-        <v>44</v>
-      </c>
-      <c r="I11">
-        <v>39</v>
-      </c>
-      <c r="J11">
-        <v>13</v>
-      </c>
-      <c r="K11">
-        <v>18</v>
-      </c>
-      <c r="M11">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -4589,29 +4526,8 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
-        <v>581</v>
-      </c>
-      <c r="G12">
-        <v>2580</v>
-      </c>
-      <c r="H12">
-        <v>1571</v>
-      </c>
-      <c r="I12">
-        <v>844</v>
-      </c>
-      <c r="J12">
-        <v>290</v>
-      </c>
-      <c r="K12">
-        <v>166</v>
-      </c>
-      <c r="M12">
-        <v>5451</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -4624,29 +4540,8 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
-        <v>577</v>
-      </c>
-      <c r="G13">
-        <v>4.0310077519379846</v>
-      </c>
-      <c r="H13">
-        <v>2.8007638446849143</v>
-      </c>
-      <c r="I13">
-        <v>4.62085308056872</v>
-      </c>
-      <c r="J13">
-        <v>4.4827586206896548</v>
-      </c>
-      <c r="K13">
-        <v>10.843373493975903</v>
-      </c>
-      <c r="M13">
-        <v>3.9992661896899651</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -4659,29 +4554,8 @@
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" t="s">
-        <v>328</v>
-      </c>
-      <c r="G14">
-        <v>1.0079368465969705</v>
-      </c>
-      <c r="H14">
-        <v>0.70031943657694806</v>
-      </c>
-      <c r="I14">
-        <v>1.1554252358798207</v>
-      </c>
-      <c r="J14">
-        <v>1.1208952863018031</v>
-      </c>
-      <c r="K14">
-        <v>2.7113407759478281</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -4695,7 +4569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -4709,7 +4583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -4722,8 +4596,11 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -4736,8 +4613,23 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>572</v>
+      </c>
+      <c r="H18" t="s">
+        <v>573</v>
+      </c>
+      <c r="I18" t="s">
+        <v>574</v>
+      </c>
+      <c r="J18" t="s">
+        <v>575</v>
+      </c>
+      <c r="K18" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -4750,8 +4642,26 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -4764,8 +4674,29 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>578</v>
+      </c>
+      <c r="G20">
+        <v>104</v>
+      </c>
+      <c r="H20">
+        <v>47</v>
+      </c>
+      <c r="I20">
+        <v>36</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+      <c r="K20">
+        <v>18</v>
+      </c>
+      <c r="M20">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -4778,8 +4709,29 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21">
+        <v>2580</v>
+      </c>
+      <c r="H21">
+        <v>1635</v>
+      </c>
+      <c r="I21">
+        <v>780</v>
+      </c>
+      <c r="J21">
+        <v>290</v>
+      </c>
+      <c r="K21">
+        <v>166</v>
+      </c>
+      <c r="M21">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -4792,8 +4744,29 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>577</v>
+      </c>
+      <c r="G22">
+        <v>4.0310077519379846</v>
+      </c>
+      <c r="H22">
+        <v>2.8746177370030579</v>
+      </c>
+      <c r="I22">
+        <v>4.6153846153846159</v>
+      </c>
+      <c r="J22">
+        <v>4.4827586206896548</v>
+      </c>
+      <c r="K22">
+        <v>10.843373493975903</v>
+      </c>
+      <c r="M22">
+        <v>3.9992661896899651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -4806,8 +4779,29 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>328</v>
+      </c>
+      <c r="G23">
+        <v>1.0079368465969705</v>
+      </c>
+      <c r="H23">
+        <v>0.71878629744970957</v>
+      </c>
+      <c r="I23">
+        <v>1.154057868736768</v>
+      </c>
+      <c r="J23">
+        <v>1.1208952863018031</v>
+      </c>
+      <c r="K23">
+        <v>2.7113407759478281</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -4821,7 +4815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -4835,7 +4829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4849,7 +4843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -4863,7 +4857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>173</v>
       </c>
@@ -4877,7 +4871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -4891,7 +4885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>175</v>
       </c>
@@ -4905,7 +4899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>176</v>
       </c>
@@ -4919,7 +4913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>177</v>
       </c>
@@ -5910,7 +5904,7 @@
         <v>8.53055364525538E-7</v>
       </c>
       <c r="D102" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -6134,7 +6128,7 @@
         <v>9.67464866885253E-9</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -6176,7 +6170,7 @@
         <v>1.48604807914394E-6</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -7560,8 +7554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDC7A97-4304-2946-827D-A013C3BEEED2}">
   <dimension ref="A1:M4294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7571,7 +7565,7 @@
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7581,8 +7575,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -7596,7 +7593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -7610,7 +7607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -7624,7 +7621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -7638,7 +7635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -7651,11 +7648,8 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7668,23 +7662,8 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>572</v>
-      </c>
-      <c r="H7" t="s">
-        <v>573</v>
-      </c>
-      <c r="I7" t="s">
-        <v>574</v>
-      </c>
-      <c r="J7" t="s">
-        <v>575</v>
-      </c>
-      <c r="K7" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>331</v>
       </c>
@@ -7697,26 +7676,8 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -7729,29 +7690,8 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>580</v>
-      </c>
-      <c r="G9">
-        <v>82</v>
-      </c>
-      <c r="H9">
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <v>51</v>
-      </c>
-      <c r="J9">
-        <v>45</v>
-      </c>
-      <c r="K9">
-        <v>26</v>
-      </c>
-      <c r="M9">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -7764,29 +7704,8 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>581</v>
-      </c>
-      <c r="G10">
-        <v>2580</v>
-      </c>
-      <c r="H10">
-        <v>1571</v>
-      </c>
-      <c r="I10">
-        <v>844</v>
-      </c>
-      <c r="J10">
-        <v>290</v>
-      </c>
-      <c r="K10">
-        <v>166</v>
-      </c>
-      <c r="M10">
-        <v>5451</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -7799,29 +7718,8 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
-        <v>577</v>
-      </c>
-      <c r="G11">
-        <v>3.1782945736434107</v>
-      </c>
-      <c r="H11">
-        <v>6.3653723742838952</v>
-      </c>
-      <c r="I11">
-        <v>6.0426540284360186</v>
-      </c>
-      <c r="J11">
-        <v>15.517241379310345</v>
-      </c>
-      <c r="K11">
-        <v>15.66265060240964</v>
-      </c>
-      <c r="M11">
-        <v>5.5769583562649059</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>334</v>
       </c>
@@ -7834,29 +7732,8 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>328</v>
-      </c>
-      <c r="G12">
-        <v>0.56989749082007335</v>
-      </c>
-      <c r="H12">
-        <v>1.1413698951388656</v>
-      </c>
-      <c r="I12">
-        <v>1.0835035233225241</v>
-      </c>
-      <c r="J12">
-        <v>2.7823843012704175</v>
-      </c>
-      <c r="K12">
-        <v>2.8084575142675967</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>335</v>
       </c>
@@ -7870,7 +7747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>336</v>
       </c>
@@ -7884,7 +7761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -7898,7 +7775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -7911,8 +7788,11 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>338</v>
       </c>
@@ -7925,8 +7805,23 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>572</v>
+      </c>
+      <c r="H17" t="s">
+        <v>573</v>
+      </c>
+      <c r="I17" t="s">
+        <v>574</v>
+      </c>
+      <c r="J17" t="s">
+        <v>575</v>
+      </c>
+      <c r="K17" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>339</v>
       </c>
@@ -7939,8 +7834,26 @@
       <c r="D18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>340</v>
       </c>
@@ -7953,8 +7866,29 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>578</v>
+      </c>
+      <c r="G19">
+        <v>82</v>
+      </c>
+      <c r="H19">
+        <v>102</v>
+      </c>
+      <c r="I19">
+        <v>49</v>
+      </c>
+      <c r="J19">
+        <v>45</v>
+      </c>
+      <c r="K19">
+        <v>26</v>
+      </c>
+      <c r="M19">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -7967,8 +7901,29 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20">
+        <v>2580</v>
+      </c>
+      <c r="H20">
+        <v>1635</v>
+      </c>
+      <c r="I20">
+        <v>780</v>
+      </c>
+      <c r="J20">
+        <v>290</v>
+      </c>
+      <c r="K20">
+        <v>166</v>
+      </c>
+      <c r="M20">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>341</v>
       </c>
@@ -7981,8 +7936,29 @@
       <c r="D21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>577</v>
+      </c>
+      <c r="G21">
+        <v>3.1782945736434107</v>
+      </c>
+      <c r="H21">
+        <v>6.238532110091743</v>
+      </c>
+      <c r="I21">
+        <v>6.2820512820512819</v>
+      </c>
+      <c r="J21">
+        <v>15.517241379310345</v>
+      </c>
+      <c r="K21">
+        <v>15.66265060240964</v>
+      </c>
+      <c r="M21">
+        <v>5.5769583562649059</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>342</v>
       </c>
@@ -7995,8 +7971,29 @@
       <c r="D22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>328</v>
+      </c>
+      <c r="G22">
+        <v>0.56989749082007335</v>
+      </c>
+      <c r="H22">
+        <v>1.1186262675036214</v>
+      </c>
+      <c r="I22">
+        <v>1.1264296558704452</v>
+      </c>
+      <c r="J22">
+        <v>2.7823843012704175</v>
+      </c>
+      <c r="K22">
+        <v>2.8084575142675967</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>343</v>
       </c>
@@ -8010,7 +8007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>344</v>
       </c>
@@ -8024,7 +8021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>345</v>
       </c>
@@ -8038,7 +8035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -8052,7 +8049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>346</v>
       </c>
@@ -8066,7 +8063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -8080,7 +8077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>348</v>
       </c>
@@ -8094,7 +8091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -8108,7 +8105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>349</v>
       </c>
@@ -8122,7 +8119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -9701,7 +9698,7 @@
         <v>8.17190687509674E-7</v>
       </c>
       <c r="D144" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -9715,7 +9712,7 @@
         <v>1.00873843633449E-7</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>